<commit_message>
update table numbers to reflect the manuscript, change alpha to italicized a in chlorophyll a
</commit_message>
<xml_diff>
--- a/tables/Appendix Table S2_NoSpores_TP_SEM_output.xlsx
+++ b/tables/Appendix Table S2_NoSpores_TP_SEM_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/Rachel Bag Experiment SEM/Data and Code/nutrient-bag-expt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{45A6CF58-704C-41D9-80B3-935F67AF9357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C941CEDC-A5E7-4E87-8123-A800081039DD}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{45A6CF58-704C-41D9-80B3-935F67AF9357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B540C9C2-49C0-43F8-920D-6B51036C0EB0}"/>
   <bookViews>
-    <workbookView xWindow="31170" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{06C333AE-A643-4FB8-BAEC-51390C8A6FB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06C333AE-A643-4FB8-BAEC-51390C8A6FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Estimate</t>
   </si>
@@ -90,27 +90,44 @@
     <t>Total Host Density</t>
   </si>
   <si>
+    <t>Mixing Treatment</t>
+  </si>
+  <si>
+    <t>Total Phosphorus</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Edible Chlorophyll </t>
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>α</t>
+      <t>a</t>
     </r>
   </si>
   <si>
-    <t>Mixing Treatment</t>
-  </si>
-  <si>
-    <t>Total Phosphorus</t>
-  </si>
-  <si>
-    <t>&lt;0.001</t>
+    <r>
+      <t xml:space="preserve">Edible Chlorophyll </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -120,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,15 +163,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +269,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,70 +287,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D22F5C-BEF1-4DFB-856A-E51EBDD022A5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7748588" y="371475"/>
-          <a:ext cx="6462712" cy="1109663"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -627,7 +591,7 @@
   <dimension ref="B2:K8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +643,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" s="16">
         <v>-1.8279298336588898E-2</v>
@@ -711,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="15">
         <v>0.31156827282590199</v>
@@ -736,10 +700,10 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="8">
         <v>0.14889951519441699</v>
@@ -757,7 +721,7 @@
         <v>7.0992511971488499</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>3</v>
@@ -768,10 +732,10 @@
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="D7" s="13">
         <v>0.614298602312075</v>
@@ -799,6 +763,6 @@
     <row r="8" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>